<commit_message>
Adding Canadian Province Data
</commit_message>
<xml_diff>
--- a/HUC_08_Inventory.xlsx
+++ b/HUC_08_Inventory.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10926"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA_Percentile_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF81608C-2114-C64A-B901-463734543391}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF45D25-C3A4-3C4B-BE52-CDA9068C884C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1360" yWindow="1400" windowWidth="24360" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16300" yWindow="460" windowWidth="24360" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HUC08_MRB_LUT" sheetId="4" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Status!$A$1:$D$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -20223,7 +20224,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -20277,16 +20278,16 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="19">
-      <c r="A4" s="11">
+      <c r="A4" s="9">
         <v>1003</v>
       </c>
-      <c r="B4" s="11">
+      <c r="B4" s="9">
         <v>10</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>1080</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>2822</v>
       </c>
     </row>
@@ -20319,16 +20320,16 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="19">
-      <c r="A7" s="11">
+      <c r="A7" s="9">
         <v>1004</v>
       </c>
-      <c r="B7" s="11">
+      <c r="B7" s="9">
         <v>11</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>1081</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="9" t="s">
         <v>2823</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding R scripts Merging of RCP Rdata Files
</commit_message>
<xml_diff>
--- a/HUC_08_Inventory.xlsx
+++ b/HUC_08_Inventory.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA_Percentile_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEF45D25-C3A4-3C4B-BE52-CDA9068C884C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50F371C2-01C7-514E-A4FC-EA0C53C6E183}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16300" yWindow="460" windowWidth="24360" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7360" yWindow="1380" windowWidth="24360" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HUC08_MRB_LUT" sheetId="4" r:id="rId1"/>
@@ -20,11 +20,10 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Big List of Names'!$A$1:$B$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HUC08_MRB_LUT!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">HUC08_MRB_LUT!$A$1:$K$308</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Status!$A$1:$D$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -9101,10 +9100,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A82313-A821-9C41-A6EE-3DE4378C62D7}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K308"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110:C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -9157,7 +9157,7 @@
         <v>2818</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" hidden="1">
       <c r="A2">
         <v>10020001</v>
       </c>
@@ -9193,7 +9193,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" hidden="1">
       <c r="A3">
         <v>10020002</v>
       </c>
@@ -9229,7 +9229,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" hidden="1">
       <c r="A4">
         <v>10020003</v>
       </c>
@@ -9265,7 +9265,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" hidden="1">
       <c r="A5">
         <v>10020004</v>
       </c>
@@ -9301,7 +9301,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" hidden="1">
       <c r="A6">
         <v>10020005</v>
       </c>
@@ -9337,7 +9337,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" hidden="1">
       <c r="A7">
         <v>10020006</v>
       </c>
@@ -9373,7 +9373,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" hidden="1">
       <c r="A8">
         <v>10020007</v>
       </c>
@@ -9409,7 +9409,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" hidden="1">
       <c r="A9">
         <v>10020008</v>
       </c>
@@ -9445,7 +9445,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" hidden="1">
       <c r="A10">
         <v>10030101</v>
       </c>
@@ -9481,7 +9481,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" hidden="1">
       <c r="A11">
         <v>10030102</v>
       </c>
@@ -9517,7 +9517,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" hidden="1">
       <c r="A12">
         <v>10030103</v>
       </c>
@@ -9553,7 +9553,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" hidden="1">
       <c r="A13">
         <v>10030104</v>
       </c>
@@ -9589,7 +9589,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" hidden="1">
       <c r="A14">
         <v>10030105</v>
       </c>
@@ -9625,7 +9625,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" hidden="1">
       <c r="A15">
         <v>10030201</v>
       </c>
@@ -9661,7 +9661,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" hidden="1">
       <c r="A16">
         <v>10030202</v>
       </c>
@@ -9697,7 +9697,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" hidden="1">
       <c r="A17">
         <v>10030203</v>
       </c>
@@ -9733,7 +9733,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" hidden="1">
       <c r="A18">
         <v>10030204</v>
       </c>
@@ -9769,7 +9769,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" hidden="1">
       <c r="A19">
         <v>10030205</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" hidden="1">
       <c r="A20">
         <v>10040101</v>
       </c>
@@ -9841,7 +9841,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" hidden="1">
       <c r="A21">
         <v>10040102</v>
       </c>
@@ -9877,7 +9877,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" hidden="1">
       <c r="A22">
         <v>10040103</v>
       </c>
@@ -9913,7 +9913,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" hidden="1">
       <c r="A23">
         <v>10040104</v>
       </c>
@@ -9949,7 +9949,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" hidden="1">
       <c r="A24">
         <v>10040105</v>
       </c>
@@ -9985,7 +9985,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" hidden="1">
       <c r="A25">
         <v>10040106</v>
       </c>
@@ -10021,7 +10021,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" hidden="1">
       <c r="A26">
         <v>10040201</v>
       </c>
@@ -10057,7 +10057,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" hidden="1">
       <c r="A27">
         <v>10040202</v>
       </c>
@@ -10093,7 +10093,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" hidden="1">
       <c r="A28">
         <v>10040203</v>
       </c>
@@ -10129,7 +10129,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" hidden="1">
       <c r="A29">
         <v>10040204</v>
       </c>
@@ -10165,7 +10165,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" hidden="1">
       <c r="A30">
         <v>10040205</v>
       </c>
@@ -10201,7 +10201,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" hidden="1">
       <c r="A31">
         <v>10050001</v>
       </c>
@@ -10237,7 +10237,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" hidden="1">
       <c r="A32">
         <v>10050002</v>
       </c>
@@ -10273,7 +10273,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" hidden="1">
       <c r="A33">
         <v>10050003</v>
       </c>
@@ -10309,7 +10309,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" hidden="1">
       <c r="A34">
         <v>10050004</v>
       </c>
@@ -10345,7 +10345,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" hidden="1">
       <c r="A35">
         <v>10050005</v>
       </c>
@@ -10381,7 +10381,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" hidden="1">
       <c r="A36">
         <v>10050006</v>
       </c>
@@ -10417,7 +10417,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" hidden="1">
       <c r="A37">
         <v>10050007</v>
       </c>
@@ -10453,7 +10453,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" hidden="1">
       <c r="A38">
         <v>10050008</v>
       </c>
@@ -10489,7 +10489,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" hidden="1">
       <c r="A39">
         <v>10050009</v>
       </c>
@@ -10525,7 +10525,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" hidden="1">
       <c r="A40">
         <v>10050010</v>
       </c>
@@ -10561,7 +10561,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" hidden="1">
       <c r="A41">
         <v>10050011</v>
       </c>
@@ -10597,7 +10597,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" hidden="1">
       <c r="A42">
         <v>10050012</v>
       </c>
@@ -10633,7 +10633,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" hidden="1">
       <c r="A43">
         <v>10050013</v>
       </c>
@@ -10669,7 +10669,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" hidden="1">
       <c r="A44">
         <v>10050014</v>
       </c>
@@ -10705,7 +10705,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" hidden="1">
       <c r="A45">
         <v>10050015</v>
       </c>
@@ -10741,7 +10741,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" hidden="1">
       <c r="A46">
         <v>10050016</v>
       </c>
@@ -10777,7 +10777,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" hidden="1">
       <c r="A47">
         <v>10060001</v>
       </c>
@@ -10813,7 +10813,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" hidden="1">
       <c r="A48">
         <v>10060002</v>
       </c>
@@ -10849,7 +10849,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" hidden="1">
       <c r="A49">
         <v>10060003</v>
       </c>
@@ -10885,7 +10885,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" hidden="1">
       <c r="A50">
         <v>10060004</v>
       </c>
@@ -10921,7 +10921,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" hidden="1">
       <c r="A51">
         <v>10060005</v>
       </c>
@@ -10957,7 +10957,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" hidden="1">
       <c r="A52">
         <v>10060006</v>
       </c>
@@ -10993,7 +10993,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" hidden="1">
       <c r="A53">
         <v>10060007</v>
       </c>
@@ -11029,7 +11029,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" hidden="1">
       <c r="A54">
         <v>10070001</v>
       </c>
@@ -11065,7 +11065,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" hidden="1">
       <c r="A55">
         <v>10070002</v>
       </c>
@@ -11101,7 +11101,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" hidden="1">
       <c r="A56">
         <v>10070003</v>
       </c>
@@ -11137,7 +11137,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" hidden="1">
       <c r="A57">
         <v>10070004</v>
       </c>
@@ -11173,7 +11173,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" hidden="1">
       <c r="A58">
         <v>10070005</v>
       </c>
@@ -11209,7 +11209,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" hidden="1">
       <c r="A59">
         <v>10070006</v>
       </c>
@@ -11245,7 +11245,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" hidden="1">
       <c r="A60">
         <v>10070007</v>
       </c>
@@ -11281,7 +11281,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" hidden="1">
       <c r="A61">
         <v>10070008</v>
       </c>
@@ -11317,7 +11317,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" hidden="1">
       <c r="A62">
         <v>10080001</v>
       </c>
@@ -11353,7 +11353,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" hidden="1">
       <c r="A63">
         <v>10080002</v>
       </c>
@@ -11389,7 +11389,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" hidden="1">
       <c r="A64">
         <v>10080003</v>
       </c>
@@ -11425,7 +11425,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" hidden="1">
       <c r="A65">
         <v>10080004</v>
       </c>
@@ -11461,7 +11461,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" hidden="1">
       <c r="A66">
         <v>10080005</v>
       </c>
@@ -11497,7 +11497,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" hidden="1">
       <c r="A67">
         <v>10080006</v>
       </c>
@@ -11533,7 +11533,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" hidden="1">
       <c r="A68">
         <v>10080007</v>
       </c>
@@ -11569,7 +11569,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" hidden="1">
       <c r="A69">
         <v>10080008</v>
       </c>
@@ -11605,7 +11605,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" hidden="1">
       <c r="A70">
         <v>10080009</v>
       </c>
@@ -11641,7 +11641,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" hidden="1">
       <c r="A71">
         <v>10080010</v>
       </c>
@@ -11677,7 +11677,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" hidden="1">
       <c r="A72">
         <v>10080011</v>
       </c>
@@ -11713,7 +11713,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" hidden="1">
       <c r="A73">
         <v>10080012</v>
       </c>
@@ -11749,7 +11749,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" hidden="1">
       <c r="A74">
         <v>10080013</v>
       </c>
@@ -11785,7 +11785,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" hidden="1">
       <c r="A75">
         <v>10080014</v>
       </c>
@@ -11821,7 +11821,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" hidden="1">
       <c r="A76">
         <v>10080015</v>
       </c>
@@ -11857,7 +11857,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" hidden="1">
       <c r="A77">
         <v>10080016</v>
       </c>
@@ -11893,7 +11893,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" hidden="1">
       <c r="A78">
         <v>10090101</v>
       </c>
@@ -11929,7 +11929,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" hidden="1">
       <c r="A79">
         <v>10090102</v>
       </c>
@@ -11965,7 +11965,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" hidden="1">
       <c r="A80">
         <v>10090201</v>
       </c>
@@ -12001,7 +12001,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" hidden="1">
       <c r="A81">
         <v>10090202</v>
       </c>
@@ -12037,7 +12037,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" hidden="1">
       <c r="A82">
         <v>10090203</v>
       </c>
@@ -12073,7 +12073,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" hidden="1">
       <c r="A83">
         <v>10090204</v>
       </c>
@@ -12109,7 +12109,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" hidden="1">
       <c r="A84">
         <v>10090205</v>
       </c>
@@ -12145,7 +12145,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" hidden="1">
       <c r="A85">
         <v>10090206</v>
       </c>
@@ -12181,7 +12181,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" hidden="1">
       <c r="A86">
         <v>10090207</v>
       </c>
@@ -12217,7 +12217,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" hidden="1">
       <c r="A87">
         <v>10090208</v>
       </c>
@@ -12253,7 +12253,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" hidden="1">
       <c r="A88">
         <v>10090209</v>
       </c>
@@ -12289,7 +12289,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" hidden="1">
       <c r="A89">
         <v>10090210</v>
       </c>
@@ -12325,7 +12325,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" hidden="1">
       <c r="A90">
         <v>10100001</v>
       </c>
@@ -12361,7 +12361,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" hidden="1">
       <c r="A91">
         <v>10100002</v>
       </c>
@@ -12397,7 +12397,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" hidden="1">
       <c r="A92">
         <v>10100003</v>
       </c>
@@ -12433,7 +12433,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" hidden="1">
       <c r="A93">
         <v>10100004</v>
       </c>
@@ -12469,7 +12469,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" hidden="1">
       <c r="A94">
         <v>10100005</v>
       </c>
@@ -12505,7 +12505,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" hidden="1">
       <c r="A95">
         <v>10110101</v>
       </c>
@@ -12541,7 +12541,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" hidden="1">
       <c r="A96">
         <v>10110102</v>
       </c>
@@ -12577,7 +12577,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" hidden="1">
       <c r="A97">
         <v>10110201</v>
       </c>
@@ -12613,7 +12613,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" hidden="1">
       <c r="A98">
         <v>10110202</v>
       </c>
@@ -12649,7 +12649,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" hidden="1">
       <c r="A99">
         <v>10110203</v>
       </c>
@@ -12685,7 +12685,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" hidden="1">
       <c r="A100">
         <v>10110204</v>
       </c>
@@ -12721,7 +12721,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" hidden="1">
       <c r="A101">
         <v>10110205</v>
       </c>
@@ -13333,7 +13333,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
+    <row r="118" spans="1:11" hidden="1">
       <c r="A118">
         <v>10130101</v>
       </c>
@@ -13369,7 +13369,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:11" hidden="1">
       <c r="A119">
         <v>10130102</v>
       </c>
@@ -13405,7 +13405,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
+    <row r="120" spans="1:11" hidden="1">
       <c r="A120">
         <v>10130103</v>
       </c>
@@ -13441,7 +13441,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:11" hidden="1">
       <c r="A121">
         <v>10130104</v>
       </c>
@@ -13477,7 +13477,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:11" hidden="1">
       <c r="A122">
         <v>10130105</v>
       </c>
@@ -13513,7 +13513,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
+    <row r="123" spans="1:11" hidden="1">
       <c r="A123">
         <v>10130106</v>
       </c>
@@ -13549,7 +13549,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
+    <row r="124" spans="1:11" hidden="1">
       <c r="A124">
         <v>10130201</v>
       </c>
@@ -13585,7 +13585,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
+    <row r="125" spans="1:11" hidden="1">
       <c r="A125">
         <v>10130202</v>
       </c>
@@ -13621,7 +13621,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:11" hidden="1">
       <c r="A126">
         <v>10130203</v>
       </c>
@@ -13657,7 +13657,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="127" spans="1:11">
+    <row r="127" spans="1:11" hidden="1">
       <c r="A127">
         <v>10130204</v>
       </c>
@@ -13693,7 +13693,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="128" spans="1:11">
+    <row r="128" spans="1:11" hidden="1">
       <c r="A128">
         <v>10130205</v>
       </c>
@@ -13729,7 +13729,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="129" spans="1:11">
+    <row r="129" spans="1:11" hidden="1">
       <c r="A129">
         <v>10130206</v>
       </c>
@@ -13765,7 +13765,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="130" spans="1:11">
+    <row r="130" spans="1:11" hidden="1">
       <c r="A130">
         <v>10130301</v>
       </c>
@@ -13801,7 +13801,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="131" spans="1:11">
+    <row r="131" spans="1:11" hidden="1">
       <c r="A131">
         <v>10130302</v>
       </c>
@@ -13837,7 +13837,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
+    <row r="132" spans="1:11" hidden="1">
       <c r="A132">
         <v>10130303</v>
       </c>
@@ -13873,7 +13873,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
+    <row r="133" spans="1:11" hidden="1">
       <c r="A133">
         <v>10130304</v>
       </c>
@@ -13909,7 +13909,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" spans="1:11" hidden="1">
       <c r="A134">
         <v>10130305</v>
       </c>
@@ -13945,7 +13945,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="135" spans="1:11">
+    <row r="135" spans="1:11" hidden="1">
       <c r="A135">
         <v>10130306</v>
       </c>
@@ -13981,7 +13981,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="136" spans="1:11">
+    <row r="136" spans="1:11" hidden="1">
       <c r="A136">
         <v>10140101</v>
       </c>
@@ -14017,7 +14017,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="137" spans="1:11">
+    <row r="137" spans="1:11" hidden="1">
       <c r="A137">
         <v>10140102</v>
       </c>
@@ -14053,7 +14053,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="138" spans="1:11">
+    <row r="138" spans="1:11" hidden="1">
       <c r="A138">
         <v>10140103</v>
       </c>
@@ -14089,7 +14089,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="139" spans="1:11">
+    <row r="139" spans="1:11" hidden="1">
       <c r="A139">
         <v>10140104</v>
       </c>
@@ -14125,7 +14125,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="140" spans="1:11">
+    <row r="140" spans="1:11" hidden="1">
       <c r="A140">
         <v>10140105</v>
       </c>
@@ -14161,7 +14161,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="141" spans="1:11">
+    <row r="141" spans="1:11" hidden="1">
       <c r="A141">
         <v>10140201</v>
       </c>
@@ -14197,7 +14197,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="142" spans="1:11">
+    <row r="142" spans="1:11" hidden="1">
       <c r="A142">
         <v>10140202</v>
       </c>
@@ -14233,7 +14233,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="143" spans="1:11">
+    <row r="143" spans="1:11" hidden="1">
       <c r="A143">
         <v>10140203</v>
       </c>
@@ -14269,7 +14269,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="144" spans="1:11">
+    <row r="144" spans="1:11" hidden="1">
       <c r="A144">
         <v>10140204</v>
       </c>
@@ -14305,7 +14305,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="145" spans="1:11">
+    <row r="145" spans="1:11" hidden="1">
       <c r="A145">
         <v>10150001</v>
       </c>
@@ -14341,7 +14341,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="146" spans="1:11">
+    <row r="146" spans="1:11" hidden="1">
       <c r="A146">
         <v>10150002</v>
       </c>
@@ -14377,7 +14377,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="147" spans="1:11">
+    <row r="147" spans="1:11" hidden="1">
       <c r="A147">
         <v>10150003</v>
       </c>
@@ -14413,7 +14413,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="148" spans="1:11">
+    <row r="148" spans="1:11" hidden="1">
       <c r="A148">
         <v>10150004</v>
       </c>
@@ -14449,7 +14449,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="149" spans="1:11">
+    <row r="149" spans="1:11" hidden="1">
       <c r="A149">
         <v>10150005</v>
       </c>
@@ -14485,7 +14485,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="150" spans="1:11">
+    <row r="150" spans="1:11" hidden="1">
       <c r="A150">
         <v>10150006</v>
       </c>
@@ -14521,7 +14521,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="151" spans="1:11">
+    <row r="151" spans="1:11" hidden="1">
       <c r="A151">
         <v>10150007</v>
       </c>
@@ -14557,7 +14557,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="152" spans="1:11">
+    <row r="152" spans="1:11" hidden="1">
       <c r="A152">
         <v>10160001</v>
       </c>
@@ -14593,7 +14593,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="153" spans="1:11">
+    <row r="153" spans="1:11" hidden="1">
       <c r="A153">
         <v>10160002</v>
       </c>
@@ -14629,7 +14629,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="154" spans="1:11">
+    <row r="154" spans="1:11" hidden="1">
       <c r="A154">
         <v>10160003</v>
       </c>
@@ -14665,7 +14665,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="155" spans="1:11">
+    <row r="155" spans="1:11" hidden="1">
       <c r="A155">
         <v>10160004</v>
       </c>
@@ -14701,7 +14701,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="156" spans="1:11">
+    <row r="156" spans="1:11" hidden="1">
       <c r="A156">
         <v>10160005</v>
       </c>
@@ -14737,7 +14737,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="157" spans="1:11">
+    <row r="157" spans="1:11" hidden="1">
       <c r="A157">
         <v>10160006</v>
       </c>
@@ -14773,7 +14773,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="158" spans="1:11">
+    <row r="158" spans="1:11" hidden="1">
       <c r="A158">
         <v>10160007</v>
       </c>
@@ -14809,7 +14809,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="159" spans="1:11">
+    <row r="159" spans="1:11" hidden="1">
       <c r="A159">
         <v>10160008</v>
       </c>
@@ -14845,7 +14845,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="160" spans="1:11">
+    <row r="160" spans="1:11" hidden="1">
       <c r="A160">
         <v>10160009</v>
       </c>
@@ -14881,7 +14881,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="161" spans="1:11">
+    <row r="161" spans="1:11" hidden="1">
       <c r="A161">
         <v>10160011</v>
       </c>
@@ -14917,7 +14917,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="162" spans="1:11">
+    <row r="162" spans="1:11" hidden="1">
       <c r="A162">
         <v>10170101</v>
       </c>
@@ -14953,7 +14953,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="163" spans="1:11">
+    <row r="163" spans="1:11" hidden="1">
       <c r="A163">
         <v>10170102</v>
       </c>
@@ -14989,7 +14989,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="164" spans="1:11">
+    <row r="164" spans="1:11" hidden="1">
       <c r="A164">
         <v>10170103</v>
       </c>
@@ -15025,7 +15025,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="165" spans="1:11">
+    <row r="165" spans="1:11" hidden="1">
       <c r="A165">
         <v>10170201</v>
       </c>
@@ -15061,7 +15061,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="166" spans="1:11">
+    <row r="166" spans="1:11" hidden="1">
       <c r="A166">
         <v>10170202</v>
       </c>
@@ -15097,7 +15097,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="167" spans="1:11">
+    <row r="167" spans="1:11" hidden="1">
       <c r="A167">
         <v>10170203</v>
       </c>
@@ -15133,7 +15133,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="168" spans="1:11">
+    <row r="168" spans="1:11" hidden="1">
       <c r="A168">
         <v>10170204</v>
       </c>
@@ -15169,7 +15169,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="169" spans="1:11">
+    <row r="169" spans="1:11" hidden="1">
       <c r="A169">
         <v>10180001</v>
       </c>
@@ -15205,7 +15205,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="170" spans="1:11">
+    <row r="170" spans="1:11" hidden="1">
       <c r="A170">
         <v>10180002</v>
       </c>
@@ -15241,7 +15241,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="171" spans="1:11">
+    <row r="171" spans="1:11" hidden="1">
       <c r="A171">
         <v>10180003</v>
       </c>
@@ -15277,7 +15277,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="172" spans="1:11">
+    <row r="172" spans="1:11" hidden="1">
       <c r="A172">
         <v>10180004</v>
       </c>
@@ -15313,7 +15313,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="173" spans="1:11">
+    <row r="173" spans="1:11" hidden="1">
       <c r="A173">
         <v>10180005</v>
       </c>
@@ -15349,7 +15349,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="174" spans="1:11">
+    <row r="174" spans="1:11" hidden="1">
       <c r="A174">
         <v>10180006</v>
       </c>
@@ -15385,7 +15385,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="175" spans="1:11">
+    <row r="175" spans="1:11" hidden="1">
       <c r="A175">
         <v>10180007</v>
       </c>
@@ -15421,7 +15421,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="176" spans="1:11">
+    <row r="176" spans="1:11" hidden="1">
       <c r="A176">
         <v>10180008</v>
       </c>
@@ -15457,7 +15457,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="177" spans="1:11">
+    <row r="177" spans="1:11" hidden="1">
       <c r="A177">
         <v>10180009</v>
       </c>
@@ -15493,7 +15493,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="178" spans="1:11">
+    <row r="178" spans="1:11" hidden="1">
       <c r="A178">
         <v>10180010</v>
       </c>
@@ -15529,7 +15529,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="179" spans="1:11">
+    <row r="179" spans="1:11" hidden="1">
       <c r="A179">
         <v>10180011</v>
       </c>
@@ -15565,7 +15565,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="180" spans="1:11">
+    <row r="180" spans="1:11" hidden="1">
       <c r="A180">
         <v>10180012</v>
       </c>
@@ -15601,7 +15601,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="181" spans="1:11">
+    <row r="181" spans="1:11" hidden="1">
       <c r="A181">
         <v>10180013</v>
       </c>
@@ -15637,7 +15637,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="182" spans="1:11">
+    <row r="182" spans="1:11" hidden="1">
       <c r="A182">
         <v>10180014</v>
       </c>
@@ -15673,7 +15673,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="183" spans="1:11">
+    <row r="183" spans="1:11" hidden="1">
       <c r="A183">
         <v>10190001</v>
       </c>
@@ -15709,7 +15709,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="184" spans="1:11">
+    <row r="184" spans="1:11" hidden="1">
       <c r="A184">
         <v>10190002</v>
       </c>
@@ -15745,7 +15745,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="185" spans="1:11">
+    <row r="185" spans="1:11" hidden="1">
       <c r="A185">
         <v>10190003</v>
       </c>
@@ -15781,7 +15781,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="186" spans="1:11">
+    <row r="186" spans="1:11" hidden="1">
       <c r="A186">
         <v>10190004</v>
       </c>
@@ -15817,7 +15817,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="187" spans="1:11">
+    <row r="187" spans="1:11" hidden="1">
       <c r="A187">
         <v>10190005</v>
       </c>
@@ -15853,7 +15853,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="188" spans="1:11">
+    <row r="188" spans="1:11" hidden="1">
       <c r="A188">
         <v>10190006</v>
       </c>
@@ -15889,7 +15889,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="189" spans="1:11">
+    <row r="189" spans="1:11" hidden="1">
       <c r="A189">
         <v>10190007</v>
       </c>
@@ -15925,7 +15925,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="190" spans="1:11">
+    <row r="190" spans="1:11" hidden="1">
       <c r="A190">
         <v>10190008</v>
       </c>
@@ -15961,7 +15961,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="191" spans="1:11">
+    <row r="191" spans="1:11" hidden="1">
       <c r="A191">
         <v>10190009</v>
       </c>
@@ -15997,7 +15997,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="192" spans="1:11">
+    <row r="192" spans="1:11" hidden="1">
       <c r="A192">
         <v>10190010</v>
       </c>
@@ -16033,7 +16033,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="193" spans="1:11">
+    <row r="193" spans="1:11" hidden="1">
       <c r="A193">
         <v>10190011</v>
       </c>
@@ -16069,7 +16069,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="194" spans="1:11">
+    <row r="194" spans="1:11" hidden="1">
       <c r="A194">
         <v>10190012</v>
       </c>
@@ -16105,7 +16105,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="195" spans="1:11">
+    <row r="195" spans="1:11" hidden="1">
       <c r="A195">
         <v>10190013</v>
       </c>
@@ -16141,7 +16141,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="196" spans="1:11">
+    <row r="196" spans="1:11" hidden="1">
       <c r="A196">
         <v>10190014</v>
       </c>
@@ -16177,7 +16177,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="197" spans="1:11">
+    <row r="197" spans="1:11" hidden="1">
       <c r="A197">
         <v>10190015</v>
       </c>
@@ -16213,7 +16213,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="198" spans="1:11">
+    <row r="198" spans="1:11" hidden="1">
       <c r="A198">
         <v>10190016</v>
       </c>
@@ -16249,7 +16249,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="199" spans="1:11">
+    <row r="199" spans="1:11" hidden="1">
       <c r="A199">
         <v>10190017</v>
       </c>
@@ -16285,7 +16285,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="200" spans="1:11">
+    <row r="200" spans="1:11" hidden="1">
       <c r="A200">
         <v>10190018</v>
       </c>
@@ -16321,7 +16321,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="201" spans="1:11">
+    <row r="201" spans="1:11" hidden="1">
       <c r="A201">
         <v>10200101</v>
       </c>
@@ -16357,7 +16357,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="202" spans="1:11">
+    <row r="202" spans="1:11" hidden="1">
       <c r="A202">
         <v>10200102</v>
       </c>
@@ -16393,7 +16393,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="203" spans="1:11">
+    <row r="203" spans="1:11" hidden="1">
       <c r="A203">
         <v>10200103</v>
       </c>
@@ -16429,7 +16429,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="204" spans="1:11">
+    <row r="204" spans="1:11" hidden="1">
       <c r="A204">
         <v>10200201</v>
       </c>
@@ -16465,7 +16465,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="205" spans="1:11">
+    <row r="205" spans="1:11" hidden="1">
       <c r="A205">
         <v>10200202</v>
       </c>
@@ -16501,7 +16501,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="206" spans="1:11">
+    <row r="206" spans="1:11" hidden="1">
       <c r="A206">
         <v>10200203</v>
       </c>
@@ -16537,7 +16537,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="207" spans="1:11">
+    <row r="207" spans="1:11" hidden="1">
       <c r="A207">
         <v>10210001</v>
       </c>
@@ -16573,7 +16573,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="208" spans="1:11">
+    <row r="208" spans="1:11" hidden="1">
       <c r="A208">
         <v>10210002</v>
       </c>
@@ -16609,7 +16609,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="209" spans="1:11">
+    <row r="209" spans="1:11" hidden="1">
       <c r="A209">
         <v>10210003</v>
       </c>
@@ -16645,7 +16645,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="210" spans="1:11">
+    <row r="210" spans="1:11" hidden="1">
       <c r="A210">
         <v>10210004</v>
       </c>
@@ -16681,7 +16681,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="211" spans="1:11">
+    <row r="211" spans="1:11" hidden="1">
       <c r="A211">
         <v>10210005</v>
       </c>
@@ -16717,7 +16717,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="212" spans="1:11">
+    <row r="212" spans="1:11" hidden="1">
       <c r="A212">
         <v>10210006</v>
       </c>
@@ -16753,7 +16753,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="213" spans="1:11">
+    <row r="213" spans="1:11" hidden="1">
       <c r="A213">
         <v>10210007</v>
       </c>
@@ -16789,7 +16789,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="214" spans="1:11">
+    <row r="214" spans="1:11" hidden="1">
       <c r="A214">
         <v>10210008</v>
       </c>
@@ -16825,7 +16825,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="215" spans="1:11">
+    <row r="215" spans="1:11" hidden="1">
       <c r="A215">
         <v>10210009</v>
       </c>
@@ -16861,7 +16861,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="216" spans="1:11">
+    <row r="216" spans="1:11" hidden="1">
       <c r="A216">
         <v>10210010</v>
       </c>
@@ -16897,7 +16897,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="217" spans="1:11">
+    <row r="217" spans="1:11" hidden="1">
       <c r="A217">
         <v>10220001</v>
       </c>
@@ -16933,7 +16933,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="218" spans="1:11">
+    <row r="218" spans="1:11" hidden="1">
       <c r="A218">
         <v>10220002</v>
       </c>
@@ -16969,7 +16969,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="219" spans="1:11">
+    <row r="219" spans="1:11" hidden="1">
       <c r="A219">
         <v>10220003</v>
       </c>
@@ -17005,7 +17005,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="220" spans="1:11">
+    <row r="220" spans="1:11" hidden="1">
       <c r="A220">
         <v>10220004</v>
       </c>
@@ -17041,7 +17041,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="221" spans="1:11">
+    <row r="221" spans="1:11" hidden="1">
       <c r="A221">
         <v>10230001</v>
       </c>
@@ -17077,7 +17077,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="222" spans="1:11">
+    <row r="222" spans="1:11" hidden="1">
       <c r="A222">
         <v>10230002</v>
       </c>
@@ -17113,7 +17113,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="223" spans="1:11">
+    <row r="223" spans="1:11" hidden="1">
       <c r="A223">
         <v>10230003</v>
       </c>
@@ -17149,7 +17149,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="224" spans="1:11">
+    <row r="224" spans="1:11" hidden="1">
       <c r="A224">
         <v>10230004</v>
       </c>
@@ -17185,7 +17185,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="225" spans="1:11">
+    <row r="225" spans="1:11" hidden="1">
       <c r="A225">
         <v>10230005</v>
       </c>
@@ -17221,7 +17221,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="226" spans="1:11">
+    <row r="226" spans="1:11" hidden="1">
       <c r="A226">
         <v>10230006</v>
       </c>
@@ -17257,7 +17257,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="227" spans="1:11">
+    <row r="227" spans="1:11" hidden="1">
       <c r="A227">
         <v>10230007</v>
       </c>
@@ -17293,7 +17293,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="228" spans="1:11">
+    <row r="228" spans="1:11" hidden="1">
       <c r="A228">
         <v>10240001</v>
       </c>
@@ -17329,7 +17329,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="229" spans="1:11">
+    <row r="229" spans="1:11" hidden="1">
       <c r="A229">
         <v>10240002</v>
       </c>
@@ -17365,7 +17365,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="230" spans="1:11">
+    <row r="230" spans="1:11" hidden="1">
       <c r="A230">
         <v>10240003</v>
       </c>
@@ -17401,7 +17401,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="231" spans="1:11">
+    <row r="231" spans="1:11" hidden="1">
       <c r="A231">
         <v>10240004</v>
       </c>
@@ -17437,7 +17437,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="232" spans="1:11">
+    <row r="232" spans="1:11" hidden="1">
       <c r="A232">
         <v>10240005</v>
       </c>
@@ -17473,7 +17473,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="233" spans="1:11">
+    <row r="233" spans="1:11" hidden="1">
       <c r="A233">
         <v>10240006</v>
       </c>
@@ -17509,7 +17509,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="234" spans="1:11">
+    <row r="234" spans="1:11" hidden="1">
       <c r="A234">
         <v>10240007</v>
       </c>
@@ -17545,7 +17545,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="235" spans="1:11">
+    <row r="235" spans="1:11" hidden="1">
       <c r="A235">
         <v>10240008</v>
       </c>
@@ -17581,7 +17581,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="236" spans="1:11">
+    <row r="236" spans="1:11" hidden="1">
       <c r="A236">
         <v>10240009</v>
       </c>
@@ -17617,7 +17617,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="237" spans="1:11">
+    <row r="237" spans="1:11" hidden="1">
       <c r="A237">
         <v>10240010</v>
       </c>
@@ -17653,7 +17653,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="238" spans="1:11">
+    <row r="238" spans="1:11" hidden="1">
       <c r="A238">
         <v>10240011</v>
       </c>
@@ -17689,7 +17689,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="239" spans="1:11">
+    <row r="239" spans="1:11" hidden="1">
       <c r="A239">
         <v>10240012</v>
       </c>
@@ -17725,7 +17725,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="240" spans="1:11">
+    <row r="240" spans="1:11" hidden="1">
       <c r="A240">
         <v>10240013</v>
       </c>
@@ -17761,7 +17761,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="241" spans="1:11">
+    <row r="241" spans="1:11" hidden="1">
       <c r="A241">
         <v>10250001</v>
       </c>
@@ -17797,7 +17797,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="242" spans="1:11">
+    <row r="242" spans="1:11" hidden="1">
       <c r="A242">
         <v>10250002</v>
       </c>
@@ -17833,7 +17833,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="243" spans="1:11">
+    <row r="243" spans="1:11" hidden="1">
       <c r="A243">
         <v>10250003</v>
       </c>
@@ -17869,7 +17869,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="244" spans="1:11">
+    <row r="244" spans="1:11" hidden="1">
       <c r="A244">
         <v>10250004</v>
       </c>
@@ -17905,7 +17905,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="245" spans="1:11">
+    <row r="245" spans="1:11" hidden="1">
       <c r="A245">
         <v>10250005</v>
       </c>
@@ -17941,7 +17941,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="246" spans="1:11">
+    <row r="246" spans="1:11" hidden="1">
       <c r="A246">
         <v>10250006</v>
       </c>
@@ -17977,7 +17977,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="247" spans="1:11">
+    <row r="247" spans="1:11" hidden="1">
       <c r="A247">
         <v>10250007</v>
       </c>
@@ -18013,7 +18013,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="248" spans="1:11">
+    <row r="248" spans="1:11" hidden="1">
       <c r="A248">
         <v>10250008</v>
       </c>
@@ -18049,7 +18049,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="249" spans="1:11">
+    <row r="249" spans="1:11" hidden="1">
       <c r="A249">
         <v>10250009</v>
       </c>
@@ -18085,7 +18085,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="250" spans="1:11">
+    <row r="250" spans="1:11" hidden="1">
       <c r="A250">
         <v>10250010</v>
       </c>
@@ -18121,7 +18121,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="251" spans="1:11">
+    <row r="251" spans="1:11" hidden="1">
       <c r="A251">
         <v>10250011</v>
       </c>
@@ -18157,7 +18157,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="252" spans="1:11">
+    <row r="252" spans="1:11" hidden="1">
       <c r="A252">
         <v>10250012</v>
       </c>
@@ -18193,7 +18193,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="253" spans="1:11">
+    <row r="253" spans="1:11" hidden="1">
       <c r="A253">
         <v>10250013</v>
       </c>
@@ -18229,7 +18229,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="254" spans="1:11">
+    <row r="254" spans="1:11" hidden="1">
       <c r="A254">
         <v>10250014</v>
       </c>
@@ -18265,7 +18265,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="255" spans="1:11">
+    <row r="255" spans="1:11" hidden="1">
       <c r="A255">
         <v>10250015</v>
       </c>
@@ -18301,7 +18301,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="256" spans="1:11">
+    <row r="256" spans="1:11" hidden="1">
       <c r="A256">
         <v>10250016</v>
       </c>
@@ -18337,7 +18337,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="257" spans="1:11">
+    <row r="257" spans="1:11" hidden="1">
       <c r="A257">
         <v>10250017</v>
       </c>
@@ -18373,7 +18373,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="258" spans="1:11">
+    <row r="258" spans="1:11" hidden="1">
       <c r="A258">
         <v>10260001</v>
       </c>
@@ -18409,7 +18409,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="259" spans="1:11">
+    <row r="259" spans="1:11" hidden="1">
       <c r="A259">
         <v>10260002</v>
       </c>
@@ -18445,7 +18445,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="260" spans="1:11">
+    <row r="260" spans="1:11" hidden="1">
       <c r="A260">
         <v>10260003</v>
       </c>
@@ -18481,7 +18481,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="261" spans="1:11">
+    <row r="261" spans="1:11" hidden="1">
       <c r="A261">
         <v>10260004</v>
       </c>
@@ -18517,7 +18517,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="262" spans="1:11">
+    <row r="262" spans="1:11" hidden="1">
       <c r="A262">
         <v>10260005</v>
       </c>
@@ -18553,7 +18553,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="263" spans="1:11">
+    <row r="263" spans="1:11" hidden="1">
       <c r="A263">
         <v>10260006</v>
       </c>
@@ -18589,7 +18589,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="264" spans="1:11">
+    <row r="264" spans="1:11" hidden="1">
       <c r="A264">
         <v>10260007</v>
       </c>
@@ -18625,7 +18625,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="265" spans="1:11">
+    <row r="265" spans="1:11" hidden="1">
       <c r="A265">
         <v>10260008</v>
       </c>
@@ -18661,7 +18661,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="266" spans="1:11">
+    <row r="266" spans="1:11" hidden="1">
       <c r="A266">
         <v>10260009</v>
       </c>
@@ -18697,7 +18697,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="267" spans="1:11">
+    <row r="267" spans="1:11" hidden="1">
       <c r="A267">
         <v>10260010</v>
       </c>
@@ -18733,7 +18733,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="268" spans="1:11">
+    <row r="268" spans="1:11" hidden="1">
       <c r="A268">
         <v>10260011</v>
       </c>
@@ -18769,7 +18769,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="269" spans="1:11">
+    <row r="269" spans="1:11" hidden="1">
       <c r="A269">
         <v>10260012</v>
       </c>
@@ -18805,7 +18805,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="270" spans="1:11">
+    <row r="270" spans="1:11" hidden="1">
       <c r="A270">
         <v>10260013</v>
       </c>
@@ -18841,7 +18841,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="271" spans="1:11">
+    <row r="271" spans="1:11" hidden="1">
       <c r="A271">
         <v>10260014</v>
       </c>
@@ -18877,7 +18877,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="272" spans="1:11">
+    <row r="272" spans="1:11" hidden="1">
       <c r="A272">
         <v>10260015</v>
       </c>
@@ -18913,7 +18913,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="273" spans="1:11">
+    <row r="273" spans="1:11" hidden="1">
       <c r="A273">
         <v>10270101</v>
       </c>
@@ -18949,7 +18949,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="274" spans="1:11">
+    <row r="274" spans="1:11" hidden="1">
       <c r="A274">
         <v>10270102</v>
       </c>
@@ -18985,7 +18985,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="275" spans="1:11">
+    <row r="275" spans="1:11" hidden="1">
       <c r="A275">
         <v>10270103</v>
       </c>
@@ -19021,7 +19021,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="276" spans="1:11">
+    <row r="276" spans="1:11" hidden="1">
       <c r="A276">
         <v>10270104</v>
       </c>
@@ -19057,7 +19057,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="277" spans="1:11">
+    <row r="277" spans="1:11" hidden="1">
       <c r="A277">
         <v>10270201</v>
       </c>
@@ -19093,7 +19093,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="278" spans="1:11">
+    <row r="278" spans="1:11" hidden="1">
       <c r="A278">
         <v>10270202</v>
       </c>
@@ -19129,7 +19129,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="279" spans="1:11">
+    <row r="279" spans="1:11" hidden="1">
       <c r="A279">
         <v>10270203</v>
       </c>
@@ -19165,7 +19165,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="280" spans="1:11">
+    <row r="280" spans="1:11" hidden="1">
       <c r="A280">
         <v>10270204</v>
       </c>
@@ -19201,7 +19201,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="281" spans="1:11">
+    <row r="281" spans="1:11" hidden="1">
       <c r="A281">
         <v>10270205</v>
       </c>
@@ -19237,7 +19237,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="282" spans="1:11">
+    <row r="282" spans="1:11" hidden="1">
       <c r="A282">
         <v>10270206</v>
       </c>
@@ -19273,7 +19273,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="283" spans="1:11">
+    <row r="283" spans="1:11" hidden="1">
       <c r="A283">
         <v>10270207</v>
       </c>
@@ -19309,7 +19309,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="284" spans="1:11">
+    <row r="284" spans="1:11" hidden="1">
       <c r="A284">
         <v>10280101</v>
       </c>
@@ -19345,7 +19345,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="285" spans="1:11">
+    <row r="285" spans="1:11" hidden="1">
       <c r="A285">
         <v>10280102</v>
       </c>
@@ -19381,7 +19381,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="286" spans="1:11">
+    <row r="286" spans="1:11" hidden="1">
       <c r="A286">
         <v>10280103</v>
       </c>
@@ -19417,7 +19417,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="287" spans="1:11">
+    <row r="287" spans="1:11" hidden="1">
       <c r="A287">
         <v>10280201</v>
       </c>
@@ -19453,7 +19453,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="288" spans="1:11">
+    <row r="288" spans="1:11" hidden="1">
       <c r="A288">
         <v>10280202</v>
       </c>
@@ -19489,7 +19489,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="289" spans="1:11">
+    <row r="289" spans="1:11" hidden="1">
       <c r="A289">
         <v>10280203</v>
       </c>
@@ -19525,7 +19525,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="290" spans="1:11">
+    <row r="290" spans="1:11" hidden="1">
       <c r="A290">
         <v>10290101</v>
       </c>
@@ -19561,7 +19561,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="291" spans="1:11">
+    <row r="291" spans="1:11" hidden="1">
       <c r="A291">
         <v>10290102</v>
       </c>
@@ -19597,7 +19597,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="292" spans="1:11">
+    <row r="292" spans="1:11" hidden="1">
       <c r="A292">
         <v>10290103</v>
       </c>
@@ -19633,7 +19633,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="293" spans="1:11">
+    <row r="293" spans="1:11" hidden="1">
       <c r="A293">
         <v>10290104</v>
       </c>
@@ -19669,7 +19669,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="294" spans="1:11">
+    <row r="294" spans="1:11" hidden="1">
       <c r="A294">
         <v>10290105</v>
       </c>
@@ -19705,7 +19705,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="295" spans="1:11">
+    <row r="295" spans="1:11" hidden="1">
       <c r="A295">
         <v>10290106</v>
       </c>
@@ -19741,7 +19741,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="296" spans="1:11">
+    <row r="296" spans="1:11" hidden="1">
       <c r="A296">
         <v>10290107</v>
       </c>
@@ -19777,7 +19777,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="297" spans="1:11">
+    <row r="297" spans="1:11" hidden="1">
       <c r="A297">
         <v>10290108</v>
       </c>
@@ -19813,7 +19813,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="298" spans="1:11">
+    <row r="298" spans="1:11" hidden="1">
       <c r="A298">
         <v>10290109</v>
       </c>
@@ -19849,7 +19849,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="299" spans="1:11">
+    <row r="299" spans="1:11" hidden="1">
       <c r="A299">
         <v>10290110</v>
       </c>
@@ -19885,7 +19885,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="300" spans="1:11">
+    <row r="300" spans="1:11" hidden="1">
       <c r="A300">
         <v>10290111</v>
       </c>
@@ -19921,7 +19921,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="301" spans="1:11">
+    <row r="301" spans="1:11" hidden="1">
       <c r="A301">
         <v>10290201</v>
       </c>
@@ -19957,7 +19957,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="302" spans="1:11">
+    <row r="302" spans="1:11" hidden="1">
       <c r="A302">
         <v>10290202</v>
       </c>
@@ -19993,7 +19993,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="303" spans="1:11">
+    <row r="303" spans="1:11" hidden="1">
       <c r="A303">
         <v>10290203</v>
       </c>
@@ -20029,7 +20029,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="304" spans="1:11">
+    <row r="304" spans="1:11" hidden="1">
       <c r="A304">
         <v>10300101</v>
       </c>
@@ -20065,7 +20065,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="305" spans="1:11">
+    <row r="305" spans="1:11" hidden="1">
       <c r="A305">
         <v>10300102</v>
       </c>
@@ -20101,7 +20101,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="306" spans="1:11">
+    <row r="306" spans="1:11" hidden="1">
       <c r="A306">
         <v>10300103</v>
       </c>
@@ -20137,7 +20137,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="307" spans="1:11">
+    <row r="307" spans="1:11" hidden="1">
       <c r="A307">
         <v>10300104</v>
       </c>
@@ -20173,7 +20173,7 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="308" spans="1:11">
+    <row r="308" spans="1:11" hidden="1">
       <c r="A308">
         <v>10300200</v>
       </c>
@@ -20210,7 +20210,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K1" xr:uid="{AAB6001D-3482-FB4E-9076-315C65BCD595}">
+  <autoFilter ref="A1:K308" xr:uid="{AAB6001D-3482-FB4E-9076-315C65BCD595}">
+    <filterColumn colId="8">
+      <filters>
+        <filter val="Cheyenne"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K308">
       <sortCondition ref="A1:A308"/>
     </sortState>
@@ -20223,8 +20228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DEBC63E-A0CE-3342-AC1B-9EB46C2A3634}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
patch on Rdata file integration
</commit_message>
<xml_diff>
--- a/HUC_08_Inventory.xlsx
+++ b/HUC_08_Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA_Percentile_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73B0F342-EA59-7949-A688-DAB3152F7DA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33DDE5C5-6AF1-DF4C-9D8D-14EA1A9128BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="760" windowWidth="24360" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8677,14 +8677,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -20260,7 +20260,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -20268,7 +20268,7 @@
     <col min="1" max="1" width="15.1640625" style="12" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" style="12" customWidth="1"/>
     <col min="3" max="3" width="24.5" style="12" customWidth="1"/>
-    <col min="4" max="4" width="12" style="19" customWidth="1"/>
+    <col min="4" max="4" width="12" style="18" customWidth="1"/>
     <col min="5" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -20343,16 +20343,16 @@
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" s="9">
+      <c r="A6" s="11">
         <v>1015</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="11">
         <v>7</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="11" t="s">
         <v>1095</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="21" t="s">
         <v>2824</v>
       </c>
     </row>
@@ -20385,16 +20385,16 @@
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="20">
+      <c r="A9" s="19">
         <v>1002</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="19">
         <v>8</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="C9" s="19" t="s">
         <v>1893</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="20" t="s">
         <v>2820</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating for speeding up return periods
</commit_message>
<xml_diff>
--- a/HUC_08_Inventory.xlsx
+++ b/HUC_08_Inventory.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wjc/GitHub/LOCA_Percentile_Processing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF493F67-6828-8943-8B5A-FD8EDAF81100}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A6E493-DED5-9849-99A6-507C2BCE7EA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6560" yWindow="1520" windowWidth="24360" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8871,10 +8871,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A82313-A821-9C41-A6EE-3DE4378C62D7}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K308"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B305" sqref="B305"/>
+    <sheetView tabSelected="1" zoomScale="171" workbookViewId="0">
+      <selection activeCell="G303" sqref="G303"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -8927,7 +8928,7 @@
         <v>2816</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" hidden="1">
       <c r="A2">
         <v>10020001</v>
       </c>
@@ -8963,7 +8964,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" hidden="1">
       <c r="A3">
         <v>10020002</v>
       </c>
@@ -8999,7 +9000,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" hidden="1">
       <c r="A4">
         <v>10020003</v>
       </c>
@@ -9035,7 +9036,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" hidden="1">
       <c r="A5">
         <v>10020004</v>
       </c>
@@ -9071,7 +9072,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" hidden="1">
       <c r="A6">
         <v>10020005</v>
       </c>
@@ -9107,7 +9108,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" hidden="1">
       <c r="A7">
         <v>10020006</v>
       </c>
@@ -9143,7 +9144,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" hidden="1">
       <c r="A8">
         <v>10020007</v>
       </c>
@@ -9179,7 +9180,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" hidden="1">
       <c r="A9">
         <v>10020008</v>
       </c>
@@ -9215,7 +9216,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" hidden="1">
       <c r="A10">
         <v>10030101</v>
       </c>
@@ -9251,7 +9252,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" hidden="1">
       <c r="A11">
         <v>10030102</v>
       </c>
@@ -9287,7 +9288,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" hidden="1">
       <c r="A12">
         <v>10030103</v>
       </c>
@@ -9323,7 +9324,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" hidden="1">
       <c r="A13">
         <v>10030104</v>
       </c>
@@ -9359,7 +9360,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" hidden="1">
       <c r="A14">
         <v>10030105</v>
       </c>
@@ -9395,7 +9396,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" hidden="1">
       <c r="A15">
         <v>10030201</v>
       </c>
@@ -9431,7 +9432,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" hidden="1">
       <c r="A16">
         <v>10030202</v>
       </c>
@@ -9467,7 +9468,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" hidden="1">
       <c r="A17">
         <v>10030203</v>
       </c>
@@ -9503,7 +9504,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" hidden="1">
       <c r="A18">
         <v>10030204</v>
       </c>
@@ -9539,7 +9540,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" hidden="1">
       <c r="A19">
         <v>10030205</v>
       </c>
@@ -9575,7 +9576,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" hidden="1">
       <c r="A20">
         <v>10040101</v>
       </c>
@@ -9611,7 +9612,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" hidden="1">
       <c r="A21">
         <v>10040102</v>
       </c>
@@ -9647,7 +9648,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" hidden="1">
       <c r="A22">
         <v>10040103</v>
       </c>
@@ -9683,7 +9684,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" hidden="1">
       <c r="A23">
         <v>10040104</v>
       </c>
@@ -9719,7 +9720,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" hidden="1">
       <c r="A24">
         <v>10040105</v>
       </c>
@@ -9755,7 +9756,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" hidden="1">
       <c r="A25">
         <v>10040106</v>
       </c>
@@ -9791,7 +9792,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" hidden="1">
       <c r="A26">
         <v>10040201</v>
       </c>
@@ -9827,7 +9828,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" hidden="1">
       <c r="A27">
         <v>10040202</v>
       </c>
@@ -9863,7 +9864,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" hidden="1">
       <c r="A28">
         <v>10040203</v>
       </c>
@@ -9899,7 +9900,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" hidden="1">
       <c r="A29">
         <v>10040204</v>
       </c>
@@ -9935,7 +9936,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" hidden="1">
       <c r="A30">
         <v>10040205</v>
       </c>
@@ -9971,7 +9972,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" hidden="1">
       <c r="A31">
         <v>10050001</v>
       </c>
@@ -10007,7 +10008,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" hidden="1">
       <c r="A32">
         <v>10050002</v>
       </c>
@@ -10043,7 +10044,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" hidden="1">
       <c r="A33">
         <v>10050003</v>
       </c>
@@ -10079,7 +10080,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" hidden="1">
       <c r="A34">
         <v>10050004</v>
       </c>
@@ -10115,7 +10116,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" hidden="1">
       <c r="A35">
         <v>10050005</v>
       </c>
@@ -10151,7 +10152,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" hidden="1">
       <c r="A36">
         <v>10050006</v>
       </c>
@@ -10187,7 +10188,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" hidden="1">
       <c r="A37">
         <v>10050007</v>
       </c>
@@ -10223,7 +10224,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" hidden="1">
       <c r="A38">
         <v>10050008</v>
       </c>
@@ -10259,7 +10260,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" hidden="1">
       <c r="A39">
         <v>10050009</v>
       </c>
@@ -10295,7 +10296,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" hidden="1">
       <c r="A40">
         <v>10050010</v>
       </c>
@@ -10331,7 +10332,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" hidden="1">
       <c r="A41">
         <v>10050011</v>
       </c>
@@ -10367,7 +10368,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" hidden="1">
       <c r="A42">
         <v>10050012</v>
       </c>
@@ -10403,7 +10404,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" hidden="1">
       <c r="A43">
         <v>10050013</v>
       </c>
@@ -10439,7 +10440,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" hidden="1">
       <c r="A44">
         <v>10050014</v>
       </c>
@@ -10475,7 +10476,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" hidden="1">
       <c r="A45">
         <v>10050015</v>
       </c>
@@ -10511,7 +10512,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" hidden="1">
       <c r="A46">
         <v>10050016</v>
       </c>
@@ -10547,7 +10548,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" hidden="1">
       <c r="A47">
         <v>10060001</v>
       </c>
@@ -10583,7 +10584,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
+    <row r="48" spans="1:11" hidden="1">
       <c r="A48">
         <v>10060002</v>
       </c>
@@ -10619,7 +10620,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
+    <row r="49" spans="1:11" hidden="1">
       <c r="A49">
         <v>10060003</v>
       </c>
@@ -10655,7 +10656,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
+    <row r="50" spans="1:11" hidden="1">
       <c r="A50">
         <v>10060004</v>
       </c>
@@ -10691,7 +10692,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" hidden="1">
       <c r="A51">
         <v>10060005</v>
       </c>
@@ -10727,7 +10728,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" hidden="1">
       <c r="A52">
         <v>10060006</v>
       </c>
@@ -10763,7 +10764,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" hidden="1">
       <c r="A53">
         <v>10060007</v>
       </c>
@@ -10799,7 +10800,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" hidden="1">
       <c r="A54">
         <v>10070001</v>
       </c>
@@ -10835,7 +10836,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" hidden="1">
       <c r="A55">
         <v>10070002</v>
       </c>
@@ -10871,7 +10872,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" hidden="1">
       <c r="A56">
         <v>10070003</v>
       </c>
@@ -10907,7 +10908,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" hidden="1">
       <c r="A57">
         <v>10070004</v>
       </c>
@@ -10943,7 +10944,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" hidden="1">
       <c r="A58">
         <v>10070005</v>
       </c>
@@ -10979,7 +10980,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" hidden="1">
       <c r="A59">
         <v>10070006</v>
       </c>
@@ -11015,7 +11016,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" hidden="1">
       <c r="A60">
         <v>10070007</v>
       </c>
@@ -11051,7 +11052,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" hidden="1">
       <c r="A61">
         <v>10070008</v>
       </c>
@@ -11087,7 +11088,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" hidden="1">
       <c r="A62">
         <v>10080001</v>
       </c>
@@ -11123,7 +11124,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" hidden="1">
       <c r="A63">
         <v>10080002</v>
       </c>
@@ -11159,7 +11160,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" hidden="1">
       <c r="A64">
         <v>10080003</v>
       </c>
@@ -11195,7 +11196,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" hidden="1">
       <c r="A65">
         <v>10080004</v>
       </c>
@@ -11231,7 +11232,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" hidden="1">
       <c r="A66">
         <v>10080005</v>
       </c>
@@ -11267,7 +11268,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" hidden="1">
       <c r="A67">
         <v>10080006</v>
       </c>
@@ -11303,7 +11304,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" hidden="1">
       <c r="A68">
         <v>10080007</v>
       </c>
@@ -11339,7 +11340,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" hidden="1">
       <c r="A69">
         <v>10080008</v>
       </c>
@@ -11375,7 +11376,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" hidden="1">
       <c r="A70">
         <v>10080009</v>
       </c>
@@ -11411,7 +11412,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" hidden="1">
       <c r="A71">
         <v>10080010</v>
       </c>
@@ -11447,7 +11448,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" hidden="1">
       <c r="A72">
         <v>10080011</v>
       </c>
@@ -11483,7 +11484,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
+    <row r="73" spans="1:11" hidden="1">
       <c r="A73">
         <v>10080012</v>
       </c>
@@ -11519,7 +11520,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" hidden="1">
       <c r="A74">
         <v>10080013</v>
       </c>
@@ -11555,7 +11556,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
+    <row r="75" spans="1:11" hidden="1">
       <c r="A75">
         <v>10080014</v>
       </c>
@@ -11591,7 +11592,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" hidden="1">
       <c r="A76">
         <v>10080015</v>
       </c>
@@ -11627,7 +11628,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
+    <row r="77" spans="1:11" hidden="1">
       <c r="A77">
         <v>10080016</v>
       </c>
@@ -11663,7 +11664,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" hidden="1">
       <c r="A78">
         <v>10090101</v>
       </c>
@@ -11699,7 +11700,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
+    <row r="79" spans="1:11" hidden="1">
       <c r="A79">
         <v>10090102</v>
       </c>
@@ -11735,7 +11736,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" hidden="1">
       <c r="A80">
         <v>10090201</v>
       </c>
@@ -11771,7 +11772,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" hidden="1">
       <c r="A81">
         <v>10090202</v>
       </c>
@@ -11807,7 +11808,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" hidden="1">
       <c r="A82">
         <v>10090203</v>
       </c>
@@ -11843,7 +11844,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" hidden="1">
       <c r="A83">
         <v>10090204</v>
       </c>
@@ -11879,7 +11880,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" hidden="1">
       <c r="A84">
         <v>10090205</v>
       </c>
@@ -11915,7 +11916,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" hidden="1">
       <c r="A85">
         <v>10090206</v>
       </c>
@@ -11951,7 +11952,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" hidden="1">
       <c r="A86">
         <v>10090207</v>
       </c>
@@ -11987,7 +11988,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" hidden="1">
       <c r="A87">
         <v>10090208</v>
       </c>
@@ -12023,7 +12024,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" hidden="1">
       <c r="A88">
         <v>10090209</v>
       </c>
@@ -12059,7 +12060,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" hidden="1">
       <c r="A89">
         <v>10090210</v>
       </c>
@@ -12095,7 +12096,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" hidden="1">
       <c r="A90">
         <v>10100001</v>
       </c>
@@ -12131,7 +12132,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" hidden="1">
       <c r="A91">
         <v>10100002</v>
       </c>
@@ -12167,7 +12168,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" hidden="1">
       <c r="A92">
         <v>10100003</v>
       </c>
@@ -12203,7 +12204,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" hidden="1">
       <c r="A93">
         <v>10100004</v>
       </c>
@@ -12239,7 +12240,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
+    <row r="94" spans="1:11" hidden="1">
       <c r="A94">
         <v>10100005</v>
       </c>
@@ -12275,7 +12276,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" hidden="1">
       <c r="A95">
         <v>10110101</v>
       </c>
@@ -12311,7 +12312,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" hidden="1">
       <c r="A96">
         <v>10110102</v>
       </c>
@@ -12347,7 +12348,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="97" spans="1:11">
+    <row r="97" spans="1:11" hidden="1">
       <c r="A97">
         <v>10110201</v>
       </c>
@@ -12383,7 +12384,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="98" spans="1:11">
+    <row r="98" spans="1:11" hidden="1">
       <c r="A98">
         <v>10110202</v>
       </c>
@@ -12419,7 +12420,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="99" spans="1:11">
+    <row r="99" spans="1:11" hidden="1">
       <c r="A99">
         <v>10110203</v>
       </c>
@@ -12455,7 +12456,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="100" spans="1:11">
+    <row r="100" spans="1:11" hidden="1">
       <c r="A100">
         <v>10110204</v>
       </c>
@@ -12491,7 +12492,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="101" spans="1:11">
+    <row r="101" spans="1:11" hidden="1">
       <c r="A101">
         <v>10110205</v>
       </c>
@@ -12527,7 +12528,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="102" spans="1:11">
+    <row r="102" spans="1:11" hidden="1">
       <c r="A102">
         <v>10120101</v>
       </c>
@@ -12563,7 +12564,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="103" spans="1:11">
+    <row r="103" spans="1:11" hidden="1">
       <c r="A103">
         <v>10120102</v>
       </c>
@@ -12599,7 +12600,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="104" spans="1:11">
+    <row r="104" spans="1:11" hidden="1">
       <c r="A104">
         <v>10120103</v>
       </c>
@@ -12635,7 +12636,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="105" spans="1:11">
+    <row r="105" spans="1:11" hidden="1">
       <c r="A105">
         <v>10120104</v>
       </c>
@@ -12671,7 +12672,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="106" spans="1:11">
+    <row r="106" spans="1:11" hidden="1">
       <c r="A106">
         <v>10120105</v>
       </c>
@@ -12707,7 +12708,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="107" spans="1:11">
+    <row r="107" spans="1:11" hidden="1">
       <c r="A107">
         <v>10120106</v>
       </c>
@@ -12743,7 +12744,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="108" spans="1:11">
+    <row r="108" spans="1:11" hidden="1">
       <c r="A108">
         <v>10120107</v>
       </c>
@@ -12779,7 +12780,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="109" spans="1:11">
+    <row r="109" spans="1:11" hidden="1">
       <c r="A109">
         <v>10120108</v>
       </c>
@@ -12815,7 +12816,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="110" spans="1:11">
+    <row r="110" spans="1:11" hidden="1">
       <c r="A110">
         <v>10120109</v>
       </c>
@@ -12851,7 +12852,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="111" spans="1:11">
+    <row r="111" spans="1:11" hidden="1">
       <c r="A111">
         <v>10120110</v>
       </c>
@@ -12887,7 +12888,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="112" spans="1:11">
+    <row r="112" spans="1:11" hidden="1">
       <c r="A112">
         <v>10120111</v>
       </c>
@@ -12923,7 +12924,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="113" spans="1:11">
+    <row r="113" spans="1:11" hidden="1">
       <c r="A113">
         <v>10120112</v>
       </c>
@@ -12959,7 +12960,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="114" spans="1:11">
+    <row r="114" spans="1:11" hidden="1">
       <c r="A114">
         <v>10120113</v>
       </c>
@@ -12995,7 +12996,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="115" spans="1:11">
+    <row r="115" spans="1:11" hidden="1">
       <c r="A115">
         <v>10120201</v>
       </c>
@@ -13031,7 +13032,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="116" spans="1:11">
+    <row r="116" spans="1:11" hidden="1">
       <c r="A116">
         <v>10120202</v>
       </c>
@@ -13067,7 +13068,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="117" spans="1:11">
+    <row r="117" spans="1:11" hidden="1">
       <c r="A117">
         <v>10120203</v>
       </c>
@@ -13103,7 +13104,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="118" spans="1:11">
+    <row r="118" spans="1:11" hidden="1">
       <c r="A118">
         <v>10130101</v>
       </c>
@@ -13139,7 +13140,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="119" spans="1:11">
+    <row r="119" spans="1:11" hidden="1">
       <c r="A119">
         <v>10130102</v>
       </c>
@@ -13175,7 +13176,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
+    <row r="120" spans="1:11" hidden="1">
       <c r="A120">
         <v>10130103</v>
       </c>
@@ -13211,7 +13212,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
+    <row r="121" spans="1:11" hidden="1">
       <c r="A121">
         <v>10130104</v>
       </c>
@@ -13247,7 +13248,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
+    <row r="122" spans="1:11" hidden="1">
       <c r="A122">
         <v>10130105</v>
       </c>
@@ -13283,7 +13284,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
+    <row r="123" spans="1:11" hidden="1">
       <c r="A123">
         <v>10130106</v>
       </c>
@@ -13319,7 +13320,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
+    <row r="124" spans="1:11" hidden="1">
       <c r="A124">
         <v>10130201</v>
       </c>
@@ -13355,7 +13356,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
+    <row r="125" spans="1:11" hidden="1">
       <c r="A125">
         <v>10130202</v>
       </c>
@@ -13391,7 +13392,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
+    <row r="126" spans="1:11" hidden="1">
       <c r="A126">
         <v>10130203</v>
       </c>
@@ -13427,7 +13428,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="127" spans="1:11">
+    <row r="127" spans="1:11" hidden="1">
       <c r="A127">
         <v>10130204</v>
       </c>
@@ -13463,7 +13464,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="128" spans="1:11">
+    <row r="128" spans="1:11" hidden="1">
       <c r="A128">
         <v>10130205</v>
       </c>
@@ -13499,7 +13500,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="129" spans="1:11">
+    <row r="129" spans="1:11" hidden="1">
       <c r="A129">
         <v>10130206</v>
       </c>
@@ -13535,7 +13536,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="130" spans="1:11">
+    <row r="130" spans="1:11" hidden="1">
       <c r="A130">
         <v>10130301</v>
       </c>
@@ -13571,7 +13572,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="131" spans="1:11">
+    <row r="131" spans="1:11" hidden="1">
       <c r="A131">
         <v>10130302</v>
       </c>
@@ -13607,7 +13608,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
+    <row r="132" spans="1:11" hidden="1">
       <c r="A132">
         <v>10130303</v>
       </c>
@@ -13643,7 +13644,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
+    <row r="133" spans="1:11" hidden="1">
       <c r="A133">
         <v>10130304</v>
       </c>
@@ -13679,7 +13680,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="134" spans="1:11">
+    <row r="134" spans="1:11" hidden="1">
       <c r="A134">
         <v>10130305</v>
       </c>
@@ -13715,7 +13716,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="135" spans="1:11">
+    <row r="135" spans="1:11" hidden="1">
       <c r="A135">
         <v>10130306</v>
       </c>
@@ -13751,7 +13752,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="136" spans="1:11">
+    <row r="136" spans="1:11" hidden="1">
       <c r="A136">
         <v>10140101</v>
       </c>
@@ -13787,7 +13788,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="137" spans="1:11">
+    <row r="137" spans="1:11" hidden="1">
       <c r="A137">
         <v>10140102</v>
       </c>
@@ -13823,7 +13824,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="138" spans="1:11">
+    <row r="138" spans="1:11" hidden="1">
       <c r="A138">
         <v>10140103</v>
       </c>
@@ -13859,7 +13860,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="139" spans="1:11">
+    <row r="139" spans="1:11" hidden="1">
       <c r="A139">
         <v>10140104</v>
       </c>
@@ -13895,7 +13896,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="140" spans="1:11">
+    <row r="140" spans="1:11" hidden="1">
       <c r="A140">
         <v>10140105</v>
       </c>
@@ -13931,7 +13932,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="141" spans="1:11">
+    <row r="141" spans="1:11" hidden="1">
       <c r="A141">
         <v>10140201</v>
       </c>
@@ -13967,7 +13968,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="142" spans="1:11">
+    <row r="142" spans="1:11" hidden="1">
       <c r="A142">
         <v>10140202</v>
       </c>
@@ -14003,7 +14004,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="143" spans="1:11">
+    <row r="143" spans="1:11" hidden="1">
       <c r="A143">
         <v>10140203</v>
       </c>
@@ -14039,7 +14040,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="144" spans="1:11">
+    <row r="144" spans="1:11" hidden="1">
       <c r="A144">
         <v>10140204</v>
       </c>
@@ -14075,7 +14076,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="145" spans="1:11">
+    <row r="145" spans="1:11" hidden="1">
       <c r="A145">
         <v>10150001</v>
       </c>
@@ -14111,7 +14112,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="146" spans="1:11">
+    <row r="146" spans="1:11" hidden="1">
       <c r="A146">
         <v>10150002</v>
       </c>
@@ -14147,7 +14148,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="147" spans="1:11">
+    <row r="147" spans="1:11" hidden="1">
       <c r="A147">
         <v>10150003</v>
       </c>
@@ -14183,7 +14184,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="148" spans="1:11">
+    <row r="148" spans="1:11" hidden="1">
       <c r="A148">
         <v>10150004</v>
       </c>
@@ -14219,7 +14220,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="149" spans="1:11">
+    <row r="149" spans="1:11" hidden="1">
       <c r="A149">
         <v>10150005</v>
       </c>
@@ -14255,7 +14256,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="150" spans="1:11">
+    <row r="150" spans="1:11" hidden="1">
       <c r="A150">
         <v>10150006</v>
       </c>
@@ -14291,7 +14292,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="151" spans="1:11">
+    <row r="151" spans="1:11" hidden="1">
       <c r="A151">
         <v>10150007</v>
       </c>
@@ -14327,7 +14328,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="152" spans="1:11">
+    <row r="152" spans="1:11" hidden="1">
       <c r="A152">
         <v>10160001</v>
       </c>
@@ -14363,7 +14364,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="153" spans="1:11">
+    <row r="153" spans="1:11" hidden="1">
       <c r="A153">
         <v>10160002</v>
       </c>
@@ -14399,7 +14400,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="154" spans="1:11">
+    <row r="154" spans="1:11" hidden="1">
       <c r="A154">
         <v>10160003</v>
       </c>
@@ -14435,7 +14436,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="155" spans="1:11">
+    <row r="155" spans="1:11" hidden="1">
       <c r="A155">
         <v>10160004</v>
       </c>
@@ -14471,7 +14472,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="156" spans="1:11">
+    <row r="156" spans="1:11" hidden="1">
       <c r="A156">
         <v>10160005</v>
       </c>
@@ -14507,7 +14508,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="157" spans="1:11">
+    <row r="157" spans="1:11" hidden="1">
       <c r="A157">
         <v>10160006</v>
       </c>
@@ -14543,7 +14544,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="158" spans="1:11">
+    <row r="158" spans="1:11" hidden="1">
       <c r="A158">
         <v>10160007</v>
       </c>
@@ -14579,7 +14580,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="159" spans="1:11">
+    <row r="159" spans="1:11" hidden="1">
       <c r="A159">
         <v>10160008</v>
       </c>
@@ -14615,7 +14616,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="160" spans="1:11">
+    <row r="160" spans="1:11" hidden="1">
       <c r="A160">
         <v>10160009</v>
       </c>
@@ -14651,7 +14652,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="161" spans="1:11">
+    <row r="161" spans="1:11" hidden="1">
       <c r="A161">
         <v>10160011</v>
       </c>
@@ -14687,7 +14688,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="162" spans="1:11">
+    <row r="162" spans="1:11" hidden="1">
       <c r="A162">
         <v>10170101</v>
       </c>
@@ -14723,7 +14724,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="163" spans="1:11">
+    <row r="163" spans="1:11" hidden="1">
       <c r="A163">
         <v>10170102</v>
       </c>
@@ -14759,7 +14760,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="164" spans="1:11">
+    <row r="164" spans="1:11" hidden="1">
       <c r="A164">
         <v>10170103</v>
       </c>
@@ -14795,7 +14796,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="165" spans="1:11">
+    <row r="165" spans="1:11" hidden="1">
       <c r="A165">
         <v>10170201</v>
       </c>
@@ -14831,7 +14832,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="166" spans="1:11">
+    <row r="166" spans="1:11" hidden="1">
       <c r="A166">
         <v>10170202</v>
       </c>
@@ -14867,7 +14868,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="167" spans="1:11">
+    <row r="167" spans="1:11" hidden="1">
       <c r="A167">
         <v>10170203</v>
       </c>
@@ -14903,7 +14904,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="168" spans="1:11">
+    <row r="168" spans="1:11" hidden="1">
       <c r="A168">
         <v>10170204</v>
       </c>
@@ -14939,7 +14940,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="169" spans="1:11">
+    <row r="169" spans="1:11" hidden="1">
       <c r="A169">
         <v>10180001</v>
       </c>
@@ -14975,7 +14976,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="170" spans="1:11">
+    <row r="170" spans="1:11" hidden="1">
       <c r="A170">
         <v>10180002</v>
       </c>
@@ -15011,7 +15012,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="171" spans="1:11">
+    <row r="171" spans="1:11" hidden="1">
       <c r="A171">
         <v>10180003</v>
       </c>
@@ -15047,7 +15048,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="172" spans="1:11">
+    <row r="172" spans="1:11" hidden="1">
       <c r="A172">
         <v>10180004</v>
       </c>
@@ -15083,7 +15084,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="173" spans="1:11">
+    <row r="173" spans="1:11" hidden="1">
       <c r="A173">
         <v>10180005</v>
       </c>
@@ -15119,7 +15120,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="174" spans="1:11">
+    <row r="174" spans="1:11" hidden="1">
       <c r="A174">
         <v>10180006</v>
       </c>
@@ -15155,7 +15156,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="175" spans="1:11">
+    <row r="175" spans="1:11" hidden="1">
       <c r="A175">
         <v>10180007</v>
       </c>
@@ -15191,7 +15192,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="176" spans="1:11">
+    <row r="176" spans="1:11" hidden="1">
       <c r="A176">
         <v>10180008</v>
       </c>
@@ -15227,7 +15228,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="177" spans="1:11">
+    <row r="177" spans="1:11" hidden="1">
       <c r="A177">
         <v>10180009</v>
       </c>
@@ -15263,7 +15264,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="178" spans="1:11">
+    <row r="178" spans="1:11" hidden="1">
       <c r="A178">
         <v>10180010</v>
       </c>
@@ -15299,7 +15300,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="179" spans="1:11">
+    <row r="179" spans="1:11" hidden="1">
       <c r="A179">
         <v>10180011</v>
       </c>
@@ -15335,7 +15336,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="180" spans="1:11">
+    <row r="180" spans="1:11" hidden="1">
       <c r="A180">
         <v>10180012</v>
       </c>
@@ -15371,7 +15372,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="181" spans="1:11">
+    <row r="181" spans="1:11" hidden="1">
       <c r="A181">
         <v>10180013</v>
       </c>
@@ -15407,7 +15408,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="182" spans="1:11">
+    <row r="182" spans="1:11" hidden="1">
       <c r="A182">
         <v>10180014</v>
       </c>
@@ -15443,7 +15444,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="183" spans="1:11">
+    <row r="183" spans="1:11" hidden="1">
       <c r="A183">
         <v>10190001</v>
       </c>
@@ -15479,7 +15480,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="184" spans="1:11">
+    <row r="184" spans="1:11" hidden="1">
       <c r="A184">
         <v>10190002</v>
       </c>
@@ -15515,7 +15516,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="185" spans="1:11">
+    <row r="185" spans="1:11" hidden="1">
       <c r="A185">
         <v>10190003</v>
       </c>
@@ -15551,7 +15552,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="186" spans="1:11">
+    <row r="186" spans="1:11" hidden="1">
       <c r="A186">
         <v>10190004</v>
       </c>
@@ -15587,7 +15588,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="187" spans="1:11">
+    <row r="187" spans="1:11" hidden="1">
       <c r="A187">
         <v>10190005</v>
       </c>
@@ -15623,7 +15624,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="188" spans="1:11">
+    <row r="188" spans="1:11" hidden="1">
       <c r="A188">
         <v>10190006</v>
       </c>
@@ -15659,7 +15660,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="189" spans="1:11">
+    <row r="189" spans="1:11" hidden="1">
       <c r="A189">
         <v>10190007</v>
       </c>
@@ -15695,7 +15696,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="190" spans="1:11">
+    <row r="190" spans="1:11" hidden="1">
       <c r="A190">
         <v>10190008</v>
       </c>
@@ -15731,7 +15732,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="191" spans="1:11">
+    <row r="191" spans="1:11" hidden="1">
       <c r="A191">
         <v>10190009</v>
       </c>
@@ -15767,7 +15768,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="192" spans="1:11">
+    <row r="192" spans="1:11" hidden="1">
       <c r="A192">
         <v>10190010</v>
       </c>
@@ -15803,7 +15804,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="193" spans="1:11">
+    <row r="193" spans="1:11" hidden="1">
       <c r="A193">
         <v>10190011</v>
       </c>
@@ -15839,7 +15840,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="194" spans="1:11">
+    <row r="194" spans="1:11" hidden="1">
       <c r="A194">
         <v>10190012</v>
       </c>
@@ -15875,7 +15876,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="195" spans="1:11">
+    <row r="195" spans="1:11" hidden="1">
       <c r="A195">
         <v>10190013</v>
       </c>
@@ -15911,7 +15912,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="196" spans="1:11">
+    <row r="196" spans="1:11" hidden="1">
       <c r="A196">
         <v>10190014</v>
       </c>
@@ -15947,7 +15948,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="197" spans="1:11">
+    <row r="197" spans="1:11" hidden="1">
       <c r="A197">
         <v>10190015</v>
       </c>
@@ -15983,7 +15984,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="198" spans="1:11">
+    <row r="198" spans="1:11" hidden="1">
       <c r="A198">
         <v>10190016</v>
       </c>
@@ -16019,7 +16020,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="199" spans="1:11">
+    <row r="199" spans="1:11" hidden="1">
       <c r="A199">
         <v>10190017</v>
       </c>
@@ -16055,7 +16056,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="200" spans="1:11">
+    <row r="200" spans="1:11" hidden="1">
       <c r="A200">
         <v>10190018</v>
       </c>
@@ -16091,7 +16092,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="201" spans="1:11">
+    <row r="201" spans="1:11" hidden="1">
       <c r="A201">
         <v>10200101</v>
       </c>
@@ -16127,7 +16128,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="202" spans="1:11">
+    <row r="202" spans="1:11" hidden="1">
       <c r="A202">
         <v>10200102</v>
       </c>
@@ -16163,7 +16164,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="203" spans="1:11">
+    <row r="203" spans="1:11" hidden="1">
       <c r="A203">
         <v>10200103</v>
       </c>
@@ -16199,7 +16200,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="204" spans="1:11">
+    <row r="204" spans="1:11" hidden="1">
       <c r="A204">
         <v>10200201</v>
       </c>
@@ -16235,7 +16236,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="205" spans="1:11">
+    <row r="205" spans="1:11" hidden="1">
       <c r="A205">
         <v>10200202</v>
       </c>
@@ -16271,7 +16272,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="206" spans="1:11">
+    <row r="206" spans="1:11" hidden="1">
       <c r="A206">
         <v>10200203</v>
       </c>
@@ -16307,7 +16308,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="207" spans="1:11">
+    <row r="207" spans="1:11" hidden="1">
       <c r="A207">
         <v>10210001</v>
       </c>
@@ -16343,7 +16344,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="208" spans="1:11">
+    <row r="208" spans="1:11" hidden="1">
       <c r="A208">
         <v>10210002</v>
       </c>
@@ -16379,7 +16380,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="209" spans="1:11">
+    <row r="209" spans="1:11" hidden="1">
       <c r="A209">
         <v>10210003</v>
       </c>
@@ -16415,7 +16416,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="210" spans="1:11">
+    <row r="210" spans="1:11" hidden="1">
       <c r="A210">
         <v>10210004</v>
       </c>
@@ -16451,7 +16452,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="211" spans="1:11">
+    <row r="211" spans="1:11" hidden="1">
       <c r="A211">
         <v>10210005</v>
       </c>
@@ -16487,7 +16488,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="212" spans="1:11">
+    <row r="212" spans="1:11" hidden="1">
       <c r="A212">
         <v>10210006</v>
       </c>
@@ -16523,7 +16524,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="213" spans="1:11">
+    <row r="213" spans="1:11" hidden="1">
       <c r="A213">
         <v>10210007</v>
       </c>
@@ -16559,7 +16560,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="214" spans="1:11">
+    <row r="214" spans="1:11" hidden="1">
       <c r="A214">
         <v>10210008</v>
       </c>
@@ -16595,7 +16596,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="215" spans="1:11">
+    <row r="215" spans="1:11" hidden="1">
       <c r="A215">
         <v>10210009</v>
       </c>
@@ -16631,7 +16632,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="216" spans="1:11">
+    <row r="216" spans="1:11" hidden="1">
       <c r="A216">
         <v>10210010</v>
       </c>
@@ -16667,7 +16668,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="217" spans="1:11">
+    <row r="217" spans="1:11" hidden="1">
       <c r="A217">
         <v>10220001</v>
       </c>
@@ -16703,7 +16704,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="218" spans="1:11">
+    <row r="218" spans="1:11" hidden="1">
       <c r="A218">
         <v>10220002</v>
       </c>
@@ -16739,7 +16740,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="219" spans="1:11">
+    <row r="219" spans="1:11" hidden="1">
       <c r="A219">
         <v>10220003</v>
       </c>
@@ -16775,7 +16776,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="220" spans="1:11">
+    <row r="220" spans="1:11" hidden="1">
       <c r="A220">
         <v>10220004</v>
       </c>
@@ -16811,7 +16812,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="221" spans="1:11">
+    <row r="221" spans="1:11" hidden="1">
       <c r="A221">
         <v>10230001</v>
       </c>
@@ -16847,7 +16848,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="222" spans="1:11">
+    <row r="222" spans="1:11" hidden="1">
       <c r="A222">
         <v>10230002</v>
       </c>
@@ -16883,7 +16884,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="223" spans="1:11">
+    <row r="223" spans="1:11" hidden="1">
       <c r="A223">
         <v>10230003</v>
       </c>
@@ -16919,7 +16920,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="224" spans="1:11">
+    <row r="224" spans="1:11" hidden="1">
       <c r="A224">
         <v>10230004</v>
       </c>
@@ -16955,7 +16956,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="225" spans="1:11">
+    <row r="225" spans="1:11" hidden="1">
       <c r="A225">
         <v>10230005</v>
       </c>
@@ -16991,7 +16992,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="226" spans="1:11">
+    <row r="226" spans="1:11" hidden="1">
       <c r="A226">
         <v>10230006</v>
       </c>
@@ -17027,7 +17028,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="227" spans="1:11">
+    <row r="227" spans="1:11" hidden="1">
       <c r="A227">
         <v>10230007</v>
       </c>
@@ -17063,7 +17064,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="228" spans="1:11">
+    <row r="228" spans="1:11" hidden="1">
       <c r="A228">
         <v>10240001</v>
       </c>
@@ -17099,7 +17100,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="229" spans="1:11">
+    <row r="229" spans="1:11" hidden="1">
       <c r="A229">
         <v>10240002</v>
       </c>
@@ -17135,7 +17136,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="230" spans="1:11">
+    <row r="230" spans="1:11" hidden="1">
       <c r="A230">
         <v>10240003</v>
       </c>
@@ -17171,7 +17172,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="231" spans="1:11">
+    <row r="231" spans="1:11" hidden="1">
       <c r="A231">
         <v>10240004</v>
       </c>
@@ -17207,7 +17208,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="232" spans="1:11">
+    <row r="232" spans="1:11" hidden="1">
       <c r="A232">
         <v>10240005</v>
       </c>
@@ -17243,7 +17244,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="233" spans="1:11">
+    <row r="233" spans="1:11" hidden="1">
       <c r="A233">
         <v>10240006</v>
       </c>
@@ -17279,7 +17280,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="234" spans="1:11">
+    <row r="234" spans="1:11" hidden="1">
       <c r="A234">
         <v>10240007</v>
       </c>
@@ -17315,7 +17316,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="235" spans="1:11">
+    <row r="235" spans="1:11" hidden="1">
       <c r="A235">
         <v>10240008</v>
       </c>
@@ -17351,7 +17352,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="236" spans="1:11">
+    <row r="236" spans="1:11" hidden="1">
       <c r="A236">
         <v>10240009</v>
       </c>
@@ -17387,7 +17388,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="237" spans="1:11">
+    <row r="237" spans="1:11" hidden="1">
       <c r="A237">
         <v>10240010</v>
       </c>
@@ -17423,7 +17424,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="238" spans="1:11">
+    <row r="238" spans="1:11" hidden="1">
       <c r="A238">
         <v>10240011</v>
       </c>
@@ -17459,7 +17460,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="239" spans="1:11">
+    <row r="239" spans="1:11" hidden="1">
       <c r="A239">
         <v>10240012</v>
       </c>
@@ -17495,7 +17496,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="240" spans="1:11">
+    <row r="240" spans="1:11" hidden="1">
       <c r="A240">
         <v>10240013</v>
       </c>
@@ -17531,7 +17532,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="241" spans="1:11">
+    <row r="241" spans="1:11" hidden="1">
       <c r="A241">
         <v>10250001</v>
       </c>
@@ -17567,7 +17568,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="242" spans="1:11">
+    <row r="242" spans="1:11" hidden="1">
       <c r="A242">
         <v>10250002</v>
       </c>
@@ -17603,7 +17604,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="243" spans="1:11">
+    <row r="243" spans="1:11" hidden="1">
       <c r="A243">
         <v>10250003</v>
       </c>
@@ -17639,7 +17640,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="244" spans="1:11">
+    <row r="244" spans="1:11" hidden="1">
       <c r="A244">
         <v>10250004</v>
       </c>
@@ -17675,7 +17676,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="245" spans="1:11">
+    <row r="245" spans="1:11" hidden="1">
       <c r="A245">
         <v>10250005</v>
       </c>
@@ -17711,7 +17712,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="246" spans="1:11">
+    <row r="246" spans="1:11" hidden="1">
       <c r="A246">
         <v>10250006</v>
       </c>
@@ -17747,7 +17748,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="247" spans="1:11">
+    <row r="247" spans="1:11" hidden="1">
       <c r="A247">
         <v>10250007</v>
       </c>
@@ -17783,7 +17784,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="248" spans="1:11">
+    <row r="248" spans="1:11" hidden="1">
       <c r="A248">
         <v>10250008</v>
       </c>
@@ -17819,7 +17820,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="249" spans="1:11">
+    <row r="249" spans="1:11" hidden="1">
       <c r="A249">
         <v>10250009</v>
       </c>
@@ -17855,7 +17856,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="250" spans="1:11">
+    <row r="250" spans="1:11" hidden="1">
       <c r="A250">
         <v>10250010</v>
       </c>
@@ -17891,7 +17892,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="251" spans="1:11">
+    <row r="251" spans="1:11" hidden="1">
       <c r="A251">
         <v>10250011</v>
       </c>
@@ -17927,7 +17928,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="252" spans="1:11">
+    <row r="252" spans="1:11" hidden="1">
       <c r="A252">
         <v>10250012</v>
       </c>
@@ -17963,7 +17964,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="253" spans="1:11">
+    <row r="253" spans="1:11" hidden="1">
       <c r="A253">
         <v>10250013</v>
       </c>
@@ -17999,7 +18000,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="254" spans="1:11">
+    <row r="254" spans="1:11" hidden="1">
       <c r="A254">
         <v>10250014</v>
       </c>
@@ -18035,7 +18036,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="255" spans="1:11">
+    <row r="255" spans="1:11" hidden="1">
       <c r="A255">
         <v>10250015</v>
       </c>
@@ -18071,7 +18072,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="256" spans="1:11">
+    <row r="256" spans="1:11" hidden="1">
       <c r="A256">
         <v>10250016</v>
       </c>
@@ -18107,7 +18108,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="257" spans="1:11">
+    <row r="257" spans="1:11" hidden="1">
       <c r="A257">
         <v>10250017</v>
       </c>
@@ -18143,7 +18144,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="258" spans="1:11">
+    <row r="258" spans="1:11" hidden="1">
       <c r="A258">
         <v>10260001</v>
       </c>
@@ -18179,7 +18180,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="259" spans="1:11">
+    <row r="259" spans="1:11" hidden="1">
       <c r="A259">
         <v>10260002</v>
       </c>
@@ -18215,7 +18216,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="260" spans="1:11">
+    <row r="260" spans="1:11" hidden="1">
       <c r="A260">
         <v>10260003</v>
       </c>
@@ -18251,7 +18252,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="261" spans="1:11">
+    <row r="261" spans="1:11" hidden="1">
       <c r="A261">
         <v>10260004</v>
       </c>
@@ -18287,7 +18288,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="262" spans="1:11">
+    <row r="262" spans="1:11" hidden="1">
       <c r="A262">
         <v>10260005</v>
       </c>
@@ -18323,7 +18324,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="263" spans="1:11">
+    <row r="263" spans="1:11" hidden="1">
       <c r="A263">
         <v>10260006</v>
       </c>
@@ -18359,7 +18360,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="264" spans="1:11">
+    <row r="264" spans="1:11" hidden="1">
       <c r="A264">
         <v>10260007</v>
       </c>
@@ -18395,7 +18396,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="265" spans="1:11">
+    <row r="265" spans="1:11" hidden="1">
       <c r="A265">
         <v>10260008</v>
       </c>
@@ -18431,7 +18432,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="266" spans="1:11">
+    <row r="266" spans="1:11" hidden="1">
       <c r="A266">
         <v>10260009</v>
       </c>
@@ -18467,7 +18468,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="267" spans="1:11">
+    <row r="267" spans="1:11" hidden="1">
       <c r="A267">
         <v>10260010</v>
       </c>
@@ -18503,7 +18504,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="268" spans="1:11">
+    <row r="268" spans="1:11" hidden="1">
       <c r="A268">
         <v>10260011</v>
       </c>
@@ -18539,7 +18540,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="269" spans="1:11">
+    <row r="269" spans="1:11" hidden="1">
       <c r="A269">
         <v>10260012</v>
       </c>
@@ -18575,7 +18576,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="270" spans="1:11">
+    <row r="270" spans="1:11" hidden="1">
       <c r="A270">
         <v>10260013</v>
       </c>
@@ -18611,7 +18612,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="271" spans="1:11">
+    <row r="271" spans="1:11" hidden="1">
       <c r="A271">
         <v>10260014</v>
       </c>
@@ -18647,7 +18648,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="272" spans="1:11">
+    <row r="272" spans="1:11" hidden="1">
       <c r="A272">
         <v>10260015</v>
       </c>
@@ -18683,7 +18684,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="273" spans="1:11">
+    <row r="273" spans="1:11" hidden="1">
       <c r="A273">
         <v>10270101</v>
       </c>
@@ -18719,7 +18720,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="274" spans="1:11">
+    <row r="274" spans="1:11" hidden="1">
       <c r="A274">
         <v>10270102</v>
       </c>
@@ -18755,7 +18756,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="275" spans="1:11">
+    <row r="275" spans="1:11" hidden="1">
       <c r="A275">
         <v>10270103</v>
       </c>
@@ -18791,7 +18792,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="276" spans="1:11">
+    <row r="276" spans="1:11" hidden="1">
       <c r="A276">
         <v>10270104</v>
       </c>
@@ -18827,7 +18828,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="277" spans="1:11">
+    <row r="277" spans="1:11" hidden="1">
       <c r="A277">
         <v>10270201</v>
       </c>
@@ -18863,7 +18864,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="278" spans="1:11">
+    <row r="278" spans="1:11" hidden="1">
       <c r="A278">
         <v>10270202</v>
       </c>
@@ -18899,7 +18900,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="279" spans="1:11">
+    <row r="279" spans="1:11" hidden="1">
       <c r="A279">
         <v>10270203</v>
       </c>
@@ -18935,7 +18936,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="280" spans="1:11">
+    <row r="280" spans="1:11" hidden="1">
       <c r="A280">
         <v>10270204</v>
       </c>
@@ -18971,7 +18972,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="281" spans="1:11">
+    <row r="281" spans="1:11" hidden="1">
       <c r="A281">
         <v>10270205</v>
       </c>
@@ -19007,7 +19008,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="282" spans="1:11">
+    <row r="282" spans="1:11" hidden="1">
       <c r="A282">
         <v>10270206</v>
       </c>
@@ -19043,7 +19044,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="283" spans="1:11">
+    <row r="283" spans="1:11" hidden="1">
       <c r="A283">
         <v>10270207</v>
       </c>
@@ -19079,7 +19080,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="284" spans="1:11">
+    <row r="284" spans="1:11" hidden="1">
       <c r="A284">
         <v>10280101</v>
       </c>
@@ -19115,7 +19116,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="285" spans="1:11">
+    <row r="285" spans="1:11" hidden="1">
       <c r="A285">
         <v>10280102</v>
       </c>
@@ -19151,7 +19152,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="286" spans="1:11">
+    <row r="286" spans="1:11" hidden="1">
       <c r="A286">
         <v>10280103</v>
       </c>
@@ -19187,7 +19188,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="287" spans="1:11">
+    <row r="287" spans="1:11" hidden="1">
       <c r="A287">
         <v>10280201</v>
       </c>
@@ -19223,7 +19224,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="288" spans="1:11">
+    <row r="288" spans="1:11" hidden="1">
       <c r="A288">
         <v>10280202</v>
       </c>
@@ -19259,7 +19260,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="289" spans="1:11">
+    <row r="289" spans="1:11" hidden="1">
       <c r="A289">
         <v>10280203</v>
       </c>
@@ -19799,7 +19800,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="304" spans="1:11">
+    <row r="304" spans="1:11" hidden="1">
       <c r="A304">
         <v>10300101</v>
       </c>
@@ -19835,7 +19836,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="305" spans="1:11">
+    <row r="305" spans="1:11" hidden="1">
       <c r="A305">
         <v>10300102</v>
       </c>
@@ -19871,7 +19872,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="306" spans="1:11">
+    <row r="306" spans="1:11" hidden="1">
       <c r="A306">
         <v>10300103</v>
       </c>
@@ -19907,7 +19908,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="307" spans="1:11">
+    <row r="307" spans="1:11" hidden="1">
       <c r="A307">
         <v>10300104</v>
       </c>
@@ -19943,7 +19944,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="308" spans="1:11">
+    <row r="308" spans="1:11" hidden="1">
       <c r="A308">
         <v>10300200</v>
       </c>
@@ -19981,6 +19982,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K308" xr:uid="{AAB6001D-3482-FB4E-9076-315C65BCD595}">
+    <filterColumn colId="7">
+      <filters>
+        <filter val="1029"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A241:K257">
       <sortCondition ref="A1:A308"/>
     </sortState>

</xml_diff>